<commit_message>
Add UNG trade, minor modification of input csv line
</commit_message>
<xml_diff>
--- a/trading data.xlsx
+++ b/trading data.xlsx
@@ -19,9 +19,6 @@
     <t>option_buy</t>
   </si>
   <si>
-    <t>20160928 +TZA-161021C27.00</t>
-  </si>
-  <si>
     <t>option_path_buy</t>
   </si>
   <si>
@@ -46,9 +43,6 @@
     <t>historical_volatility_buy</t>
   </si>
   <si>
-    <t>call</t>
-  </si>
-  <si>
     <t>expiration_yy</t>
   </si>
   <si>
@@ -64,9 +58,6 @@
     <t>entry_date_buy_mm</t>
   </si>
   <si>
-    <t>TZA</t>
-  </si>
-  <si>
     <t>option_write</t>
   </si>
   <si>
@@ -91,9 +82,6 @@
     <t>historical_volatility_write</t>
   </si>
   <si>
-    <t>20160928 +TZA-161021C26.00</t>
-  </si>
-  <si>
     <t>FIELD</t>
   </si>
   <si>
@@ -122,6 +110,18 @@
   </si>
   <si>
     <t>entry_date_write_SS</t>
+  </si>
+  <si>
+    <t>20160928 +UNG-161021P8.00</t>
+  </si>
+  <si>
+    <t>put</t>
+  </si>
+  <si>
+    <t>UNG</t>
+  </si>
+  <si>
+    <t>20160928 +UNG-161021P9.00</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,10 +500,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -511,36 +511,36 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
         <v>2016</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>10</v>
@@ -556,7 +556,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
         <v>21</v>
@@ -564,23 +564,23 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1">
-        <v>1.19</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2">
-        <v>26.885000000000002</v>
+        <v>8.5150000000000006</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>2016</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2">
         <v>9</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2">
         <v>28</v>
@@ -604,87 +604,87 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18">
-        <v>0.50970000000000004</v>
+        <v>0.3085</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22">
-        <v>-1.84</v>
+        <v>-0.65</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23">
-        <v>27.19</v>
+        <v>8.4649999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>2016</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25">
         <v>9</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>28</v>
@@ -708,34 +708,34 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B28">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B29">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B30">
-        <v>0.50970000000000004</v>
+        <v>0.3085</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add SQQ trade, add more info in buy leg results
</commit_message>
<xml_diff>
--- a/trading data.xlsx
+++ b/trading data.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="20160928 TZA" sheetId="1" r:id="rId1"/>
+    <sheet name="20160928 UNG" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>option_buy</t>
   </si>
@@ -43,6 +43,9 @@
     <t>historical_volatility_buy</t>
   </si>
   <si>
+    <t>call</t>
+  </si>
+  <si>
     <t>expiration_yy</t>
   </si>
   <si>
@@ -112,16 +115,10 @@
     <t>entry_date_write_SS</t>
   </si>
   <si>
-    <t>20160928 +UNG-161021P8.00</t>
-  </si>
-  <si>
-    <t>put</t>
-  </si>
-  <si>
-    <t>UNG</t>
-  </si>
-  <si>
-    <t>20160928 +UNG-161021P9.00</t>
+    <t>20160928 +SQQQ-161021C13.00</t>
+  </si>
+  <si>
+    <t>SQQQ</t>
   </si>
 </sst>
 </file>
@@ -489,7 +486,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,10 +497,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -511,7 +508,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -527,7 +524,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -535,12 +532,12 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
         <v>2016</v>
@@ -548,7 +545,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2">
         <v>10</v>
@@ -556,7 +553,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>21</v>
@@ -567,7 +564,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1">
-        <v>0.13</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -575,12 +572,12 @@
         <v>6</v>
       </c>
       <c r="B10" s="2">
-        <v>8.5150000000000006</v>
+        <v>13.45</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2">
         <v>2016</v>
@@ -588,7 +585,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2">
         <v>9</v>
@@ -596,7 +593,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2">
         <v>28</v>
@@ -604,26 +601,26 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="2">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -639,103 +636,67 @@
         <v>8</v>
       </c>
       <c r="B18">
-        <v>0.3085</v>
+        <v>0.43140000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22">
-        <v>-0.65</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23">
-        <v>8.4649999999999999</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24">
-        <v>2016</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30">
-        <v>0.3085</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>